<commit_message>
done for external app launcher
</commit_message>
<xml_diff>
--- a/lib/external app launcher/Android Application ID/Android Application ID.xlsx
+++ b/lib/external app launcher/Android Application ID/Android Application ID.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vscode\flutter\excel for Android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vscode\flutter\lib\external app launcher\Android Application ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91138BA0-0531-4424-8102-7D88B1646D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82A7973-CC90-4961-969E-F5315E597D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="110">
   <si>
     <t>Default platform</t>
   </si>
@@ -42,7 +42,8 @@
     <t>Color tile #</t>
   </si>
   <si>
-    <t>Youtube</t>
+    <t>Android Application ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>youtube.com</t>
@@ -120,9 +121,6 @@
     <t>open.spotify.com</t>
   </si>
   <si>
-    <t>spotify</t>
-  </si>
-  <si>
     <t>#1ED760</t>
   </si>
   <si>
@@ -154,9 +152,6 @@
   </si>
   <si>
     <t>behance.com</t>
-  </si>
-  <si>
-    <t>behance</t>
   </si>
   <si>
     <t>#1769FF</t>
@@ -252,9 +247,6 @@
     <t>producthunt.com</t>
   </si>
   <si>
-    <t>producthunt</t>
-  </si>
-  <si>
     <t>#DA552F</t>
   </si>
   <si>
@@ -296,6 +288,98 @@
   <si>
     <t>#189AF5</t>
   </si>
+  <si>
+    <t>Whatsapp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.whatsapp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.facebook.katana</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.instagram.android</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.google.android.googlequicksearchbox</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.github.android</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.google.android.youtube</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.gitlab.terrakok.gitfox</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.medium.reader</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>spotify</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.spotify.music</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>io.kodular.anujanand301201.Dribbble</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>behance</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.behance.behance</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.reddit.frontpage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>apps.secondart.stackoverflow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>producthunt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.producthuntmobile</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.W3school.offline</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Youtube</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.chrome.dev</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.sec.android.app.sbrowser</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -310,19 +394,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -331,11 +402,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,19 +456,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -415,15 +494,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="圖片 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0365973F-243C-41F3-B90B-36749BDF1111}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1DC505D-FB2B-4EAA-9321-D44E87BDFD73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -446,7 +525,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="350520"/>
+          <a:off x="3108960" y="518160"/>
           <a:ext cx="274320" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -476,15 +555,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="圖片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9F917FC-ED0D-42ED-AD58-37EBB7C7A6A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B82C01C7-1980-4EF2-A4EB-41D8A94A46E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -507,7 +586,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="739140"/>
+          <a:off x="3108960" y="906780"/>
           <a:ext cx="274320" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -537,15 +616,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="圖片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C6B188-01F3-4B8D-963D-CE0603D9F028}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD84D9C3-FDB8-4C6F-981A-41CF55C5A5A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -568,7 +647,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="1127760"/>
+          <a:off x="3108960" y="1295400"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -598,15 +677,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="圖片 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B603FC63-46F1-4B6C-A2CB-BE7E82311067}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCBF02D6-2F32-4048-BD5E-1E9011C1CD98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -629,7 +708,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="1516380"/>
+          <a:off x="3108960" y="1684020"/>
           <a:ext cx="213360" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -659,15 +738,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="圖片 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFB6F02B-55EB-4397-B537-91CA3F5FFC37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63CAEBDF-AF23-433D-A236-1CA2FF38D784}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -690,7 +769,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="1905000"/>
+          <a:off x="3108960" y="2072640"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -720,15 +799,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="圖片 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0B943F1-62EF-40C6-8A61-9948C4C37C2F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EE008FE-04AC-4745-9F7F-151A3F4B9A59}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -751,7 +830,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="2484120"/>
+          <a:off x="3108960" y="2651760"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -781,15 +860,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="圖片 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACFA24F6-3270-40F8-B225-3913B7D7BB36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97201B20-E9B5-4288-AC82-98B4F4F942E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -812,7 +891,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="2872740"/>
+          <a:off x="3108960" y="3040380"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -842,15 +921,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="圖片 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EA9B73E-82FE-4389-A5D0-AC4852B5DEDF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B8ADD0B-1160-4479-AC0B-A9C250A75ADB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -873,7 +952,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="3261360"/>
+          <a:off x="3108960" y="3429000"/>
           <a:ext cx="160020" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -903,15 +982,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="圖片 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A360164-7C9F-4E1A-AC89-3CD199DE1314}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C4D457E-FD7F-4C90-9B07-F5DE5CC41410}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -934,7 +1013,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="3840480"/>
+          <a:off x="3108960" y="4008120"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -964,15 +1043,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="圖片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3785C79-D068-4E03-BCFF-133BB322BAD5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C2EB823-E7FB-4CB1-B502-AC00E41E46F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -995,7 +1074,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="4229100"/>
+          <a:off x="3108960" y="4396740"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1025,15 +1104,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="12" name="圖片 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0574A290-674A-4E58-9798-0C7894AC4AB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9AED41D-8489-44A2-900C-0954355193E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1056,7 +1135,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="4617720"/>
+          <a:off x="3108960" y="4785360"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1086,15 +1165,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="13" name="圖片 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8B3F342-6A2B-402A-9844-1B3F5975646A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9235A78D-3262-436A-B8E1-631CEDCFBF6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1117,7 +1196,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="5006340"/>
+          <a:off x="3108960" y="5173980"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1147,15 +1226,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="14" name="圖片 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABAB89C4-872E-49B5-9ECD-1AED4352E338}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{316973BE-5AAC-4527-959E-C769C74B2499}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1178,7 +1257,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="5394960"/>
+          <a:off x="3108960" y="5562600"/>
           <a:ext cx="388620" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1208,15 +1287,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="15" name="圖片 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50661E14-0A2E-4B92-87D8-6C4CD9805F5E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB762821-2613-4585-8E0A-32CFA6A01A5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1239,7 +1318,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="5783580"/>
+          <a:off x="3108960" y="5951220"/>
           <a:ext cx="441960" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1269,15 +1348,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="16" name="圖片 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{264B7D48-23A8-4E69-8F75-E43A278EDE0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7166A939-89DF-48AB-B09E-EC534FA9E35C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1379,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="6172200"/>
+          <a:off x="3108960" y="6339840"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1330,15 +1409,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="17" name="圖片 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B087CEB7-F5B6-4E84-8C9F-F249DA73EFA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C0ADE6C-B62C-46B9-9C67-80C7C78E9B25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1361,7 +1440,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="6560820"/>
+          <a:off x="3108960" y="6728460"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1391,15 +1470,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="18" name="圖片 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1347BFCB-FDA2-4667-96AA-F77629478F86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACCE6819-EA22-492C-860E-6F24B68CB996}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,7 +1501,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="6949440"/>
+          <a:off x="3108960" y="7117080"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1452,15 +1531,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="19" name="圖片 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64A9EC3E-BBE2-433E-BC02-823D0684CCD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{738A050A-2D5A-49EC-A7D4-213F9A4D5D12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1483,7 +1562,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="7338060"/>
+          <a:off x="3108960" y="7505700"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1513,15 +1592,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="20" name="圖片 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72144CBE-DD14-470C-9E6E-654B2179B347}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B3D84AC-6BA6-443A-A254-823E0EF1C5CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1544,7 +1623,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="7726680"/>
+          <a:off x="3108960" y="7894320"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1574,15 +1653,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="21" name="圖片 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2106A8-4056-4401-93FF-BA3173E4E3B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D656C6D-10DC-4EB5-A250-89B5FE5C5546}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1605,7 +1684,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="8115300"/>
+          <a:off x="3108960" y="8282940"/>
           <a:ext cx="213360" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1643,7 +1722,7 @@
         <xdr:cNvPr id="22" name="圖片 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{540A52B6-31BC-4E46-8564-80752FEF53A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E53BCBD-193E-4AD5-857D-2CF25794855A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1666,7 +1745,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="8900160"/>
+          <a:off x="3108960" y="9067800"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1704,7 +1783,7 @@
         <xdr:cNvPr id="23" name="圖片 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF7343B-14BC-406D-9583-7AE937DC3C6D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{854DDEF5-F95D-43CF-A12D-393BF783248A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1727,7 +1806,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="9098280"/>
+          <a:off x="3108960" y="9265920"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1757,15 +1836,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="24" name="圖片 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{821D5E53-8D4B-4E5F-9CDE-3D302544C907}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18ACB499-8CE5-4E4C-997D-9D7137E55A22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1788,7 +1867,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="9296400"/>
+          <a:off x="3108960" y="9464040"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1818,15 +1897,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="25" name="圖片 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E3E2DD-D8F3-4E3D-88B7-235BE423093B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F82CD7-9B5E-404C-A2E1-C0B6BE2F6F4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1849,7 +1928,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="12390120"/>
+          <a:off x="3108960" y="12557760"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1879,15 +1958,15 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="26" name="圖片 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{996C6D70-75E7-4F55-AD71-254B434CBF51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00D3008A-E382-41F8-8952-1476A518B05A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1910,7 +1989,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1645920" y="12740640"/>
+          <a:off x="3108960" y="12908280"/>
           <a:ext cx="198120" cy="198120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2198,13 +2277,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9" style="3"/>
+    <col min="5" max="5" width="15.25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2220,7 +2308,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -2242,11 +2332,11 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2256,7 +2346,9 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2278,11 +2370,11 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2292,7 +2384,9 @@
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2314,11 +2408,11 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2328,7 +2422,9 @@
       <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2350,11 +2446,11 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2364,7 +2460,9 @@
       <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2386,11 +2484,11 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2422,11 +2520,11 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2436,7 +2534,9 @@
       <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2458,21 +2558,23 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2494,19 +2596,19 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2530,21 +2632,23 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2566,21 +2670,23 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2602,21 +2708,23 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>46</v>
+      <c r="B12" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2638,21 +2746,23 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>50</v>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2674,21 +2784,23 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>54</v>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2710,21 +2822,23 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>58</v>
+      <c r="B15" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2746,21 +2860,23 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>62</v>
+      <c r="B16" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2782,21 +2898,23 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>66</v>
+      <c r="B17" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -2818,21 +2936,23 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>70</v>
+      <c r="B18" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -2854,21 +2974,23 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>74</v>
+      <c r="B19" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -2890,21 +3012,23 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>78</v>
+      <c r="B20" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -2926,21 +3050,23 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>82</v>
+      <c r="B21" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -2963,12 +3089,16 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3020,7 +3150,7 @@
     </row>
     <row r="24" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3050,13 +3180,15 @@
     </row>
     <row r="25" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -3078,17 +3210,19 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" spans="1:26" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -3474,9 +3608,9 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
     </row>
-    <row r="40" spans="1:26" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3506,15 +3640,15 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" spans="1:26" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -30391,28 +30525,28 @@
       <c r="Z1000" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://www.youtube.com/" xr:uid="{E3B9FDFA-3EB5-4258-8680-9D8D3917C193}"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://www.medium.com/" xr:uid="{E327623D-41A7-4F1E-8A93-1338E2100581}"/>
-    <hyperlink ref="B4" r:id="rId3" display="http://github.com/" xr:uid="{C4C8C298-509F-4098-B995-DA1B59DE1CEB}"/>
-    <hyperlink ref="B5" r:id="rId4" display="http://gitlab.com/" xr:uid="{D99A05DD-DF82-4394-AA1C-9420AEEA497E}"/>
-    <hyperlink ref="B6" r:id="rId5" display="http://podcasts.apple.com/" xr:uid="{B6F2D6B0-358F-4043-B276-6EB88F345DD6}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://podcasts.google.com/" xr:uid="{576D5D4A-9C91-402C-B929-0F01FA8BAF16}"/>
-    <hyperlink ref="B8" r:id="rId7" display="http://open.spotify.com/" xr:uid="{B152F237-787B-4615-9238-0C41D3B0DDE2}"/>
-    <hyperlink ref="B9" r:id="rId8" display="http://developer.apple.com/" xr:uid="{D46E3AC1-CD12-492F-A187-22B94C652D49}"/>
-    <hyperlink ref="B10" r:id="rId9" display="http://dribbble.com/" xr:uid="{FB1DCA24-B86E-4AAA-8BD7-F7ED70D9A886}"/>
-    <hyperlink ref="B11" r:id="rId10" display="http://behance.com/" xr:uid="{1E4BC453-B3AA-4FF7-B8DA-397D8B5F03FA}"/>
-    <hyperlink ref="B12" r:id="rId11" display="http://reddit.com/" xr:uid="{51DEA37D-FDDA-4F2F-AF5B-98FBFF76D31E}"/>
-    <hyperlink ref="B13" r:id="rId12" display="http://stackoverflow.com/" xr:uid="{6186D38D-EB6F-4852-9BDB-7B4D203A895E}"/>
-    <hyperlink ref="B14" r:id="rId13" display="http://techcrunch.com/" xr:uid="{6A8138CB-3DC2-471A-9D07-41C24D9BB1D0}"/>
-    <hyperlink ref="B15" r:id="rId14" display="http://kaggle.com/" xr:uid="{E0C884D0-F7F2-4113-80B2-C929953CC1A4}"/>
-    <hyperlink ref="B16" r:id="rId15" display="http://hackernoon.com/" xr:uid="{5821868D-D51C-4A20-BA18-DF0A1C78EAD4}"/>
-    <hyperlink ref="B17" r:id="rId16" display="http://facebook.com/" xr:uid="{9621F23A-7C95-4C8A-A936-5CA0A9B5FF9C}"/>
-    <hyperlink ref="B18" r:id="rId17" display="http://instagram.com/" xr:uid="{29486701-1668-45C6-B32E-45AF9714E477}"/>
-    <hyperlink ref="B19" r:id="rId18" display="http://producthunt.com/" xr:uid="{CCCF0F34-9C39-48A7-AA92-F6A6BCC16EA7}"/>
-    <hyperlink ref="B20" r:id="rId19" display="http://geeksforgeeks.org/" xr:uid="{44D789AD-FAFE-451B-A8C9-DFE83E2E0A57}"/>
-    <hyperlink ref="B21" r:id="rId20" display="https://www.w3schools.com/" xr:uid="{8E2DC9D2-3523-451A-B929-0F8BFAF79596}"/>
+    <hyperlink ref="B21" r:id="rId1" display="https://www.w3schools.com/" xr:uid="{F8C192A4-A540-48FC-AC99-54F0953D0769}"/>
+    <hyperlink ref="B20" r:id="rId2" display="http://geeksforgeeks.org/" xr:uid="{DE96BBEB-6253-4CEF-96A5-CB5463842C26}"/>
+    <hyperlink ref="B19" r:id="rId3" display="http://producthunt.com/" xr:uid="{2B890C6D-C5FF-4F36-A449-C2498E0984C0}"/>
+    <hyperlink ref="B18" r:id="rId4" display="http://instagram.com/" xr:uid="{17C58C07-E7AE-4C9D-A0B4-D8F7043854C3}"/>
+    <hyperlink ref="B17" r:id="rId5" display="http://facebook.com/" xr:uid="{E9B9B88F-AECD-435B-9095-8291393B3EED}"/>
+    <hyperlink ref="B16" r:id="rId6" display="http://hackernoon.com/" xr:uid="{44D7D3AD-3049-42BA-B7C7-2CC6567483A4}"/>
+    <hyperlink ref="B15" r:id="rId7" display="http://kaggle.com/" xr:uid="{1E51317A-65A5-4439-B2BB-EC67766E1E3C}"/>
+    <hyperlink ref="B14" r:id="rId8" display="http://techcrunch.com/" xr:uid="{4C56BFAC-C5BA-427B-A868-538B2E37D161}"/>
+    <hyperlink ref="B13" r:id="rId9" display="http://stackoverflow.com/" xr:uid="{D873E595-A296-41C4-BADC-2FDB1171224A}"/>
+    <hyperlink ref="B12" r:id="rId10" display="http://reddit.com/" xr:uid="{7ACBFB44-247F-4116-961B-5D66DC870ADA}"/>
+    <hyperlink ref="B11" r:id="rId11" display="http://behance.com/" xr:uid="{CE4720AF-ADDC-4540-8456-BAFBBA2F4441}"/>
+    <hyperlink ref="B10" r:id="rId12" display="http://dribbble.com/" xr:uid="{2742D0CE-A8EF-4404-8971-BAE84B945ED8}"/>
+    <hyperlink ref="B9" r:id="rId13" display="http://developer.apple.com/" xr:uid="{AF3E81FA-23B0-43A5-9217-9076E7A0507B}"/>
+    <hyperlink ref="B8" r:id="rId14" display="http://open.spotify.com/" xr:uid="{2F935BB5-5189-4192-B4CC-32D963D8CD78}"/>
+    <hyperlink ref="B7" r:id="rId15" display="https://podcasts.google.com/" xr:uid="{DBA0D22A-FCDB-4F3D-93AE-501600D8061F}"/>
+    <hyperlink ref="B6" r:id="rId16" display="http://podcasts.apple.com/" xr:uid="{649497A5-A144-49BF-87CE-81F895CD23CC}"/>
+    <hyperlink ref="B5" r:id="rId17" display="http://gitlab.com/" xr:uid="{1C071C67-5024-44A1-B4A5-CCA8FB5D5056}"/>
+    <hyperlink ref="B4" r:id="rId18" display="http://github.com/" xr:uid="{40E8A601-97AA-4DCC-99F7-54F6CAD075D5}"/>
+    <hyperlink ref="B3" r:id="rId19" display="http://www.medium.com/" xr:uid="{12309C19-D5CE-4D43-B65B-23F3CE9B01F7}"/>
+    <hyperlink ref="B2" r:id="rId20" display="http://www.youtube.com/" xr:uid="{CB53CBB6-FD98-40C6-B3CB-3859BBF3F825}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>

</xml_diff>